<commit_message>
Updates for PI3K drug list
Updates for PI3K drug list
</commit_message>
<xml_diff>
--- a/required-files/inputs_file.xlsx
+++ b/required-files/inputs_file.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Beatson\negative DESI ibds and imzMLs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\2020_Scripts for Data Processing\Git Repository (March 2020)\required-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245E5875-4CC9-4A60-98A2-28E1D7CDD739}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253C799E-11B2-492F-A063-30093D4DFFBA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="-108" windowWidth="22188" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="64">
   <si>
     <t>Outputs path</t>
   </si>
@@ -217,13 +217,19 @@
   </si>
   <si>
     <t>X:\Beatson\data processing outputs ca\</t>
+  </si>
+  <si>
+    <t>U13C-glutamine SLC7a5</t>
+  </si>
+  <si>
+    <t>PI3K Drug List</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,6 +271,13 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -486,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -593,6 +606,69 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -620,67 +696,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -963,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -980,11 +999,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
       <c r="D1" s="12" t="s">
         <v>15</v>
       </c>
@@ -993,27 +1012,27 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
       <c r="D2" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
+      <c r="A3" s="57"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
       <c r="D3" s="12" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="12" t="s">
         <v>5</v>
       </c>
@@ -1022,9 +1041,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="12" t="s">
         <v>6</v>
       </c>
@@ -1033,36 +1052,36 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="12" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
       <c r="D7" s="12" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
       <c r="D8" s="12" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
       <c r="D9" s="12" t="s">
         <v>0</v>
       </c>
@@ -1071,13 +1090,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="64" t="s">
         <v>53</v>
       </c>
       <c r="D10" s="33" t="s">
@@ -1088,9 +1107,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="50"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="44"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="65"/>
       <c r="D11" s="33" t="s">
         <v>52</v>
       </c>
@@ -1099,9 +1118,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37" t="s">
+      <c r="A12" s="53"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58" t="s">
         <v>49</v>
       </c>
       <c r="D12" s="32" t="s">
@@ -1112,9 +1131,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
+      <c r="A13" s="53"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
       <c r="D13" s="32" t="s">
         <v>50</v>
       </c>
@@ -1123,9 +1142,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="50"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
+      <c r="A14" s="53"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
       <c r="D14" s="32" t="s">
         <v>51</v>
       </c>
@@ -1134,17 +1153,17 @@
       </c>
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="50"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="40" t="s">
+      <c r="A15" s="53"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="42"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="63"/>
     </row>
     <row r="16" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="50"/>
-      <c r="B16" s="37"/>
+      <c r="A16" s="53"/>
+      <c r="B16" s="58"/>
       <c r="C16" s="2" t="s">
         <v>42</v>
       </c>
@@ -1156,8 +1175,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="50"/>
-      <c r="B17" s="37"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="7" t="s">
         <v>24</v>
       </c>
@@ -1169,11 +1188,11 @@
       </c>
     </row>
     <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="50"/>
-      <c r="B18" s="39" t="s">
+      <c r="A18" s="53"/>
+      <c r="B18" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="39"/>
+      <c r="C18" s="60"/>
       <c r="D18" s="15" t="s">
         <v>19</v>
       </c>
@@ -1182,20 +1201,20 @@
       </c>
     </row>
     <row r="19" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="50"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
+      <c r="A19" s="53"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="60"/>
       <c r="D19" s="15" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="22"/>
     </row>
     <row r="20" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="50"/>
-      <c r="B20" s="38" t="s">
+      <c r="A20" s="53"/>
+      <c r="B20" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="38"/>
+      <c r="C20" s="59"/>
       <c r="D20" s="14" t="s">
         <v>19</v>
       </c>
@@ -1204,20 +1223,20 @@
       </c>
     </row>
     <row r="21" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="50"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
+      <c r="A21" s="53"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
       <c r="D21" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="23"/>
     </row>
     <row r="22" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="50"/>
-      <c r="B22" s="53" t="s">
+      <c r="A22" s="53"/>
+      <c r="B22" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="53"/>
+      <c r="C22" s="56"/>
       <c r="D22" s="16" t="s">
         <v>19</v>
       </c>
@@ -1226,9 +1245,9 @@
       </c>
     </row>
     <row r="23" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="50"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
+      <c r="A23" s="53"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
       <c r="D23" s="16" t="s">
         <v>9</v>
       </c>
@@ -1237,11 +1256,11 @@
       </c>
     </row>
     <row r="24" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="50"/>
-      <c r="B24" s="52" t="s">
+      <c r="A24" s="53"/>
+      <c r="B24" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="52"/>
+      <c r="C24" s="55"/>
       <c r="D24" s="8" t="s">
         <v>19</v>
       </c>
@@ -1250,20 +1269,20 @@
       </c>
     </row>
     <row r="25" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="50"/>
-      <c r="B25" s="52"/>
-      <c r="C25" s="52"/>
+      <c r="A25" s="53"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="55"/>
       <c r="D25" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E25" s="25"/>
     </row>
     <row r="26" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="50"/>
-      <c r="B26" s="45" t="s">
+      <c r="A26" s="53"/>
+      <c r="B26" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="46"/>
+      <c r="C26" s="49"/>
       <c r="D26" s="30" t="s">
         <v>19</v>
       </c>
@@ -1272,30 +1291,30 @@
       </c>
     </row>
     <row r="27" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="51"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="48"/>
+      <c r="A27" s="54"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="51"/>
       <c r="D27" s="30" t="s">
         <v>9</v>
       </c>
       <c r="E27" s="31"/>
     </row>
     <row r="28" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="58" t="s">
+      <c r="A28" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="60" t="s">
+      <c r="B28" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="57" t="s">
+      <c r="C28" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
     </row>
     <row r="29" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="59"/>
-      <c r="B29" s="61"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="46"/>
       <c r="C29" s="6" t="s">
         <v>17</v>
       </c>
@@ -1307,8 +1326,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="59"/>
-      <c r="B30" s="61"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="46"/>
       <c r="C30" s="6" t="s">
         <v>43</v>
       </c>
@@ -1320,8 +1339,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="59"/>
-      <c r="B31" s="61"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="46"/>
       <c r="C31" s="6" t="s">
         <v>57</v>
       </c>
@@ -1333,8 +1352,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="59"/>
-      <c r="B32" s="61"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="46"/>
       <c r="C32" s="6" t="s">
         <v>47</v>
       </c>
@@ -1346,8 +1365,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="59"/>
-      <c r="B33" s="61"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="46"/>
       <c r="C33" s="6" t="s">
         <v>46</v>
       </c>
@@ -1359,8 +1378,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="59"/>
-      <c r="B34" s="61"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="46"/>
       <c r="C34" s="6" t="s">
         <v>45</v>
       </c>
@@ -1372,8 +1391,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="59"/>
-      <c r="B35" s="61"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="46"/>
       <c r="C35" s="6" t="s">
         <v>59</v>
       </c>
@@ -1385,8 +1404,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="59"/>
-      <c r="B36" s="61"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="46"/>
       <c r="C36" s="6" t="s">
         <v>60</v>
       </c>
@@ -1397,320 +1416,337 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="5" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="59"/>
-      <c r="B37" s="61"/>
-    </row>
-    <row r="38" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="59"/>
-      <c r="B38" s="61"/>
-      <c r="C38" s="54" t="s">
+    <row r="37" spans="1:5" s="66" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="41"/>
+      <c r="B37" s="46"/>
+      <c r="C37" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="66" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="41"/>
+      <c r="B38" s="46"/>
+      <c r="C38" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="41"/>
+      <c r="B39" s="46"/>
+      <c r="C39" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="54"/>
-      <c r="E38" s="54"/>
-    </row>
-    <row r="39" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="59"/>
-      <c r="B39" s="61"/>
-      <c r="C39" s="6" t="s">
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+    </row>
+    <row r="40" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="41"/>
+      <c r="B40" s="46"/>
+      <c r="C40" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D39" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="E39" s="26" t="s">
+      <c r="D40" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="5" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="59"/>
-      <c r="B40" s="61"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-    </row>
-    <row r="41" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="59"/>
-      <c r="B41" s="61"/>
-      <c r="C41" s="54" t="s">
+    <row r="41" spans="1:5" s="5" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="41"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+    </row>
+    <row r="42" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="41"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="D41" s="54"/>
-      <c r="E41" s="54"/>
-    </row>
-    <row r="42" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="59"/>
-      <c r="B42" s="61"/>
-      <c r="C42" s="6" t="s">
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+    </row>
+    <row r="43" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="41"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E42" s="26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="59"/>
-      <c r="B43" s="61"/>
-      <c r="C43" s="6" t="s">
+      <c r="D43" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="41"/>
+      <c r="B44" s="46"/>
+      <c r="C44" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D43" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E43" s="26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="59"/>
-      <c r="B44" s="61"/>
-      <c r="C44" s="6" t="s">
+      <c r="D44" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="41"/>
+      <c r="B45" s="46"/>
+      <c r="C45" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E44" s="26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="59"/>
-      <c r="B45" s="61"/>
-      <c r="C45" s="6" t="s">
+      <c r="D45" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="41"/>
+      <c r="B46" s="46"/>
+      <c r="C46" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D45" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E45" s="26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="59"/>
-      <c r="B46" s="61"/>
-      <c r="C46" s="6" t="s">
+      <c r="D46" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="41"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D46" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E46" s="26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="59"/>
-      <c r="B47" s="61"/>
-      <c r="C47" s="6" t="s">
+      <c r="D47" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="41"/>
+      <c r="B48" s="46"/>
+      <c r="C48" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E47" s="26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="59"/>
-      <c r="B48" s="61"/>
-      <c r="C48" s="6" t="s">
+      <c r="D48" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="41"/>
+      <c r="B49" s="46"/>
+      <c r="C49" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D48" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E48" s="26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="59"/>
-      <c r="B49" s="61"/>
-      <c r="C49" s="6" t="s">
+      <c r="D49" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="41"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D49" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E49" s="26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" s="5" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A50" s="59"/>
-      <c r="B50" s="61"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-    </row>
-    <row r="51" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="59"/>
-      <c r="B51" s="62"/>
-      <c r="C51" s="54"/>
-      <c r="D51" s="54"/>
-      <c r="E51" s="54"/>
+      <c r="D50" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="5" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A51" s="41"/>
+      <c r="B51" s="46"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
     </row>
     <row r="52" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="59"/>
-      <c r="B52" s="63" t="s">
+      <c r="A52" s="41"/>
+      <c r="B52" s="47"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="38"/>
+    </row>
+    <row r="53" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="41"/>
+      <c r="B53" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="54" t="s">
+      <c r="C53" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="D52" s="12" t="s">
+      <c r="D53" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E52" s="19">
+      <c r="E53" s="19">
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="59"/>
-      <c r="B53" s="64"/>
-      <c r="C53" s="54"/>
-      <c r="D53" s="12" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="41"/>
+      <c r="B54" s="43"/>
+      <c r="C54" s="38"/>
+      <c r="D54" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E53" s="19">
+      <c r="E54" s="19">
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="59"/>
-      <c r="B54" s="64"/>
-      <c r="C54" s="56" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="41"/>
+      <c r="B55" s="43"/>
+      <c r="C55" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D54" s="11" t="str">
+      <c r="D55" s="11" t="str">
         <f>"H"</f>
         <v>H</v>
       </c>
-      <c r="E54" s="27" t="s">
+      <c r="E55" s="27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="59"/>
-      <c r="B55" s="64"/>
-      <c r="C55" s="56"/>
-      <c r="D55" s="11" t="str">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="41"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="11" t="str">
         <f>"Na"</f>
         <v>Na</v>
       </c>
-      <c r="E55" s="27" t="s">
+      <c r="E56" s="27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="59"/>
-      <c r="B56" s="64"/>
-      <c r="C56" s="56"/>
-      <c r="D56" s="11" t="str">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="41"/>
+      <c r="B57" s="43"/>
+      <c r="C57" s="37"/>
+      <c r="D57" s="11" t="str">
         <f>"K"</f>
         <v>K</v>
       </c>
-      <c r="E56" s="27" t="s">
+      <c r="E57" s="27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="59"/>
-      <c r="B57" s="64"/>
-      <c r="C57" s="56"/>
-      <c r="D57" s="11" t="str">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="41"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="11" t="str">
         <f>"-OH"</f>
         <v>-OH</v>
       </c>
-      <c r="E57" s="27" t="s">
+      <c r="E58" s="27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="59"/>
-      <c r="B58" s="64"/>
-      <c r="C58" s="56"/>
-      <c r="D58" s="11" t="str">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="41"/>
+      <c r="B59" s="43"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="11" t="str">
         <f>"H3O"</f>
         <v>H3O</v>
       </c>
-      <c r="E58" s="27" t="s">
+      <c r="E59" s="27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="59"/>
-      <c r="B59" s="64"/>
-      <c r="C59" s="56"/>
-      <c r="D59" s="11" t="str">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="41"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="37"/>
+      <c r="D60" s="11" t="str">
         <f>"NH4"</f>
         <v>NH4</v>
       </c>
-      <c r="E59" s="27" t="s">
+      <c r="E60" s="27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="59"/>
-      <c r="B60" s="64"/>
-      <c r="C60" s="55" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="41"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="D60" s="10" t="str">
+      <c r="D61" s="10" t="str">
         <f>"-H3O"</f>
         <v>-H3O</v>
       </c>
-      <c r="E60" s="28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="59"/>
-      <c r="B61" s="64"/>
-      <c r="C61" s="55"/>
-      <c r="D61" s="10" t="str">
+      <c r="E61" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="41"/>
+      <c r="B62" s="43"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="10" t="str">
         <f>"-H"</f>
         <v>-H</v>
       </c>
-      <c r="E61" s="28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="59"/>
-      <c r="B62" s="64"/>
-      <c r="C62" s="55"/>
-      <c r="D62" s="10" t="str">
+      <c r="E62" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="41"/>
+      <c r="B63" s="43"/>
+      <c r="C63" s="36"/>
+      <c r="D63" s="10" t="str">
         <f>"OH"</f>
         <v>OH</v>
       </c>
-      <c r="E62" s="28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="59"/>
-      <c r="B63" s="65"/>
-      <c r="C63" s="55"/>
-      <c r="D63" s="10" t="str">
+      <c r="E63" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="41"/>
+      <c r="B64" s="44"/>
+      <c r="C64" s="36"/>
+      <c r="D64" s="10" t="str">
         <f>"Cl"</f>
         <v>Cl</v>
       </c>
-      <c r="E63" s="28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
+      <c r="E64" s="28" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C65" s="3"/>
@@ -1752,22 +1788,13 @@
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
     </row>
+    <row r="73" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C60:C63"/>
-    <mergeCell ref="C54:C59"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="A28:A63"/>
-    <mergeCell ref="B52:B63"/>
-    <mergeCell ref="B28:B51"/>
-    <mergeCell ref="B26:C27"/>
-    <mergeCell ref="A10:A27"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="B22:C23"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C51:E51"/>
     <mergeCell ref="A1:C9"/>
     <mergeCell ref="B10:B17"/>
     <mergeCell ref="B20:C21"/>
@@ -1775,6 +1802,20 @@
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B26:C27"/>
+    <mergeCell ref="A10:A27"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C61:C64"/>
+    <mergeCell ref="C55:C60"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="A28:A64"/>
+    <mergeCell ref="B53:B64"/>
+    <mergeCell ref="B28:B52"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C52:E52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>